<commit_message>
SWOT strategy, use case
</commit_message>
<xml_diff>
--- a/doc/swotka.xlsx
+++ b/doc/swotka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silbe\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2639E5-7E2A-4095-BCA1-1902CB1C157F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D000DCF2-77C0-4F73-9A58-228F5FE5F07B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14475" xr2:uid="{9E604CB6-3EA8-43AF-86A4-B0DFC9B8B06F}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>17. Nedostatek financí pro úplnou integraci domu se systémem</t>
   </si>
   <si>
-    <t>2 + 4 / 7: Existence již zavedených čidel v domě a úspora peněz za vytápění kompenzují vysoké vstupní náklady s prvotním pořízením a zavedením systému</t>
-  </si>
-  <si>
     <t>5. Správa systému z jakéhokoliv zařízení</t>
   </si>
   <si>
@@ -102,19 +99,22 @@
     <t>14. Sledování trendů v oblasti zabezpečení IoT</t>
   </si>
   <si>
-    <t>3 + 5 / 15: Správa systému z jakéhokoliv zařízení a přehled dat na jednom místě umožňuje vyšší míru kontroly a včasného záchytu útoku zvenčí</t>
-  </si>
-  <si>
-    <t>12 + 2 / 15: Vykompenzované vstupní náklady dáky úsporám za existenci již stávajících čidel můžeme investovat do zvýšení bezpečnosti systému</t>
-  </si>
-  <si>
-    <t>14 + 7 / 16: Komparace nabídek v oblasti nových trendů zabezpečení IoT a orientace v nabídkách podpory ze strany jiných poskytovatelů(výrobců) podpory snižujeme možné riziko ukončení podpory ze strany původního výrobce. Zvyšování bezpečnosti systému nesnižuje hodnotu domu.</t>
-  </si>
-  <si>
-    <t>10 / 16 + 17: instalované solární panely mohou ušetřit energii i přes počáteční náklady, které mohou být pak investovány do upgradu nebo změny systému v případě ukončení podpory ze strany výrobce.</t>
-  </si>
-  <si>
     <t>1 / 7: Pro běžného uživatele bez hloubkových technických znalostí jsou vyšší vstupní náklady akceptovatelné, pokud zvyšují  komfort ovládání chytrého domu.</t>
+  </si>
+  <si>
+    <t>2 + 4 / 7: Existence již zavedených čidel v domě a úspora peněz za vytápění kompenzují vysoké vstupní náklady s prvotním pořízením a zavedením systému.</t>
+  </si>
+  <si>
+    <t>3 + 5 / 15: Správa systému z jakéhokoliv zařízení a přehled dat na jednom místě umožňuje vyšší míru kontroly a včasného záchytu útoku zvenčí.</t>
+  </si>
+  <si>
+    <t>10 / 16 + 17: Instalované solární panely mohou ušetřit energii i přes počáteční náklady, které mohou být pak investovány do upgradu nebo změny systému v případě ukončení podpory ze strany výrobce.</t>
+  </si>
+  <si>
+    <t>12 + 2 / 15: Vykompenzované vstupní náklady díky úsporám za existenci již stávajících čidel můžeme investovat do zvýšení bezpečnosti systému.</t>
+  </si>
+  <si>
+    <t>14 + 7 / 16: Komparace nabídek v oblasti nových trendů zabezpečení IoT a orientace v nabídkách podpory ze strany jiných poskytovatelů(výrobců) podpory můžeme snížit případné riziko ukončení podpory ze strany původního výrobce. Zvyšování bezpečnosti systému nesnižuje hodnotu domu.</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926FA5F4-A645-4A6A-9322-917D3A7CDB69}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +529,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -558,12 +558,12 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -584,7 +584,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
@@ -600,12 +600,12 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -615,32 +615,32 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>